<commit_message>
added photo showing the  registration error when leaving a field on the form blank.
</commit_message>
<xml_diff>
--- a/Completed-MoffatBayTestPlan.xlsx
+++ b/Completed-MoffatBayTestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bellevue\fifth\moffatBayCode\Moffat-Bay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3B51281-6D66-4DF7-80CA-5A4BA57FC7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B979C1A-2FA8-419B-B104-C89EB63B13B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-4425" windowWidth="29040" windowHeight="16440" xr2:uid="{EA818A59-5475-43B3-BE94-1CCE7B8A4FCE}"/>
   </bookViews>
@@ -561,16 +561,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -988,6 +988,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>286297</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>168592</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E515565-B762-7FE4-CD85-27F026204953}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13354050" y="16297275"/>
+          <a:ext cx="10649497" cy="6159817"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1310,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD18A209-C1CE-4045-BD92-60568EDDEB78}">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1385,48 +1429,48 @@
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
     </row>
     <row r="8" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="14"/>
+      <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E9" s="14"/>
+      <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="16" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="10" t="s">
@@ -1434,10 +1478,10 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="10" t="s">
         <v>6</v>
       </c>
@@ -1497,12 +1541,12 @@
       <c r="A15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
@@ -1522,36 +1566,36 @@
       <c r="A18" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
     </row>
     <row r="19" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E19" s="14"/>
+      <c r="E19" s="16"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="14"/>
+      <c r="E20" s="16"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
@@ -1642,12 +1686,12 @@
       <c r="A26" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
@@ -1667,36 +1711,36 @@
       <c r="A29" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
     </row>
     <row r="30" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="13"/>
-      <c r="B30" s="14" t="s">
+      <c r="A30" s="15"/>
+      <c r="B30" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E30" s="14"/>
+      <c r="E30" s="16"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="13"/>
-      <c r="B31" s="14"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="14"/>
+      <c r="E31" s="16"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
@@ -1770,12 +1814,12 @@
       <c r="A36" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
@@ -1795,36 +1839,36 @@
       <c r="A39" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
     </row>
     <row r="40" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="13"/>
-      <c r="B40" s="14" t="s">
+      <c r="A40" s="15"/>
+      <c r="B40" s="16" t="s">
         <v>43</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E40" s="14"/>
+      <c r="E40" s="16"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
-      <c r="B41" s="14"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="16"/>
       <c r="C41" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E41" s="14"/>
+      <c r="E41" s="16"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
@@ -1932,12 +1976,12 @@
       <c r="A48" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
@@ -1957,36 +2001,36 @@
       <c r="A51" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
     </row>
     <row r="52" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="13"/>
-      <c r="B52" s="14" t="s">
+      <c r="A52" s="15"/>
+      <c r="B52" s="16" t="s">
         <v>55</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E52" s="14"/>
+      <c r="E52" s="16"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="13"/>
-      <c r="B53" s="14"/>
+      <c r="A53" s="15"/>
+      <c r="B53" s="16"/>
       <c r="C53" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E53" s="14"/>
+      <c r="E53" s="16"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
@@ -2039,7 +2083,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="25" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="11">
         <v>3</v>
       </c>
@@ -2060,47 +2104,47 @@
       <c r="A58" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
     </row>
     <row r="61" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
     </row>
     <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="13"/>
-      <c r="B62" s="14" t="s">
+      <c r="A62" s="15"/>
+      <c r="B62" s="16" t="s">
         <v>62</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D62" s="14" t="s">
+      <c r="D62" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E62" s="14"/>
+      <c r="E62" s="16"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="13"/>
-      <c r="B63" s="14"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="16"/>
       <c r="C63" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D63" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E63" s="14"/>
+      <c r="E63" s="16"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
@@ -2208,34 +2252,20 @@
       <c r="A70" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B70" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="15"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="B70:E70"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
@@ -2252,11 +2282,25 @@
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>